<commit_message>
Prueba mas de 1 aprendiz
Se realizan pruebas y correcciones para que se revisen todos los aprendices dentro del excel y se verifiquen sus bitacoras individualmente
</commit_message>
<xml_diff>
--- a/Sources/prototiposSeguimiento.xlsx
+++ b/Sources/prototiposSeguimiento.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sena\Programacion de Software\Etapa productiva\requerimientosSenaBeta\requerimientosSenaBeta\Sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E99695-ACA3-44DE-A402-E70E0BC9B6A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A506164B-3E60-4AA8-AA8F-953AD713F6C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="78">
   <si>
     <t>TD</t>
   </si>
@@ -253,6 +253,12 @@
   </si>
   <si>
     <t>CorreoAprendiz</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>Andrés Castro</t>
   </si>
 </sst>
 </file>
@@ -562,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BD1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AA5" sqref="AA5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -771,7 +777,7 @@
         <v>1112223</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>56</v>
@@ -798,7 +804,7 @@
         <v>63</v>
       </c>
       <c r="L2" s="6">
-        <v>44743</v>
+        <v>45474</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>64</v>
@@ -843,13 +849,13 @@
         <v>71</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="AD2" s="3" t="s">
         <v>71</v>
@@ -930,6 +936,346 @@
         <v>71</v>
       </c>
       <c r="BD2" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1112223</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L3" s="6">
+        <v>45474</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE3" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AF3" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AL3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AM3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AP3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AQ3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AR3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AS3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AT3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AU3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AV3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AW3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AX3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AY3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AZ3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BA3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BB3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BC3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BD3" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1112223</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L4" s="6">
+        <v>45474</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AD4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AF4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AL4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AM4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AP4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AQ4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AR4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AS4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AT4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AU4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AV4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AW4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AX4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AY4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AZ4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BA4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BB4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BC4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BD4" s="1" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Excel y req 3
se arregla el excel para que funcione el numero total de bitacoras y el correo del instructor y se terminan las partes B y C del requerimiento 3.
</commit_message>
<xml_diff>
--- a/Sources/prototiposSeguimiento.xlsx
+++ b/Sources/prototiposSeguimiento.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sena\Programacion de Software\Etapa productiva\requerimientosSenaBeta\requerimientosSenaBeta\Sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B3A319-3A08-4892-98F7-836D13FD4617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B15162-0257-49B9-AF30-C85FD22C4510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="GkesIxTP3EaxNSguFhy4y5R3arhE8u9pZq5IxXZMqxk="/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="78">
   <si>
     <t>TD</t>
   </si>
@@ -72,12 +72,6 @@
     <t>Final_Real (Aprendiz_EP)</t>
   </si>
   <si>
-    <t>Bitácoras</t>
-  </si>
-  <si>
-    <t>Instructor Seguimiento</t>
-  </si>
-  <si>
     <t>Datos Empresa</t>
   </si>
   <si>
@@ -234,12 +228,6 @@
     <t>1900-01-01  NA</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">37505087 - MOJICA </t>
-  </si>
-  <si>
     <t>NO</t>
   </si>
   <si>
@@ -262,6 +250,15 @@
   </si>
   <si>
     <t>David Agudelo</t>
+  </si>
+  <si>
+    <t>andres_fcastrol@soy.sena.edu.co</t>
+  </si>
+  <si>
+    <t>Bitacoras</t>
+  </si>
+  <si>
+    <t>instructor_seguimiento</t>
   </si>
 </sst>
 </file>
@@ -271,11 +268,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -312,6 +316,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF323130"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -346,14 +356,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BD1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -591,8 +603,9 @@
     <col min="14" max="14" width="45.7109375" customWidth="1"/>
     <col min="15" max="15" width="21.42578125" customWidth="1"/>
     <col min="16" max="16" width="28.85546875" customWidth="1"/>
-    <col min="17" max="18" width="10.5703125" customWidth="1"/>
-    <col min="19" max="19" width="19.42578125" customWidth="1"/>
+    <col min="17" max="17" width="15.42578125" customWidth="1"/>
+    <col min="18" max="18" width="15" customWidth="1"/>
+    <col min="19" max="19" width="31.28515625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="13.5703125" customWidth="1"/>
     <col min="21" max="21" width="25.7109375" customWidth="1"/>
     <col min="22" max="22" width="16.5703125" customWidth="1"/>
@@ -622,7 +635,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
@@ -637,7 +650,7 @@
         <v>9</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>10</v>
@@ -655,632 +668,638 @@
         <v>14</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AO1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AU1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AW1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AY1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AY1" s="2" t="s">
+      <c r="BA1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="BB1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="BC1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:56" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="BD1" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="B2" s="1">
         <v>1112223</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="L2" s="6">
         <v>45474</v>
       </c>
       <c r="M2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="P2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1">
+        <f>COUNTIF(AA2:AM2, "si")</f>
+        <v>3</v>
+      </c>
+      <c r="S2" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AO2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="AP2" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="S2" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="AB2" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="AC2" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="AD2" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="AE2" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="AF2" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="AG2" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AH2" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AI2" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AJ2" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AK2" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AL2" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AM2" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AN2" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AO2" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AP2" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="AQ2" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AR2" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="AS2" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="AT2" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="AU2" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="AV2" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="AW2" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="AX2" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="AY2" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="AZ2" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="BA2" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="BB2" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="BC2" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="BD2" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B3" s="1">
         <v>1112223</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="G3" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="L3" s="6">
         <v>45474</v>
       </c>
       <c r="M3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="O3" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="P3" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q3" s="1" t="s">
+      <c r="R3" s="1">
+        <f t="shared" ref="R3:R4" si="0">COUNTIF(AA3:AM3, "si")</f>
+        <v>4</v>
+      </c>
+      <c r="S3" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AJ3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AK3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AO3" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="AP3" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="S3" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="Y3" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA3" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="AB3" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="AC3" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="AD3" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="AE3" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="AF3" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="AG3" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AH3" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AI3" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AJ3" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AK3" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AL3" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AM3" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AN3" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AO3" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AP3" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="AQ3" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AR3" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="AS3" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="AT3" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="AU3" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="AV3" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="AW3" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="AX3" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="AY3" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="AZ3" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="BA3" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="BB3" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="BC3" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="BD3" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B4" s="1">
         <v>1112223</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="G4" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="L4" s="6">
+        <v>45413</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="L4" s="6">
-        <v>45474</v>
-      </c>
-      <c r="M4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="P4" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q4" s="1" t="s">
+      <c r="R4" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S4" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC4" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD4" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE4" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF4" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AJ4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AK4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AO4" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="AP4" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="S4" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="X4" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="Y4" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="Z4" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA4" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="AB4" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="AC4" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="AD4" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="AE4" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="AF4" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="AG4" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AH4" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AI4" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AJ4" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AK4" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AL4" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AM4" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AN4" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AO4" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AP4" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="AQ4" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AR4" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="AS4" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="AT4" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="AU4" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="AV4" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="AW4" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="AX4" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="AY4" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="AZ4" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="BA4" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="BB4" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="BC4" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="BD4" s="1" t="s">
-        <v>61</v>
-      </c>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S5" s="7"/>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Requerimiento 2 y funcion correo
Se acaba requerimiento 2 que verifica la firma del acta de inicio, envia una notificacion antes de la semana y al pasar la semana se notifica comite academico. Por otro lado, se realizan dos fucniones para enviar correo al aprendiz y al instructor y de esta forma usarlas de forma recursiva en los requerimientos
</commit_message>
<xml_diff>
--- a/Sources/prototiposSeguimiento.xlsx
+++ b/Sources/prototiposSeguimiento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sena\Programacion de Software\Etapa productiva\requerimientosSenaBeta\requerimientosSenaBeta\Sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7251591-23BF-47F6-A7A8-44F4033971A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C89DAEB1-7986-42A7-951F-CE06EF6A3AF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="79">
   <si>
     <t>TD</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Alternativa (Equipo Relaciones Corporativas)</t>
   </si>
   <si>
-    <t>Alternativa (Equipo Etapa Productiva)</t>
-  </si>
-  <si>
     <t>Inicio_Ficha (Lectiva)</t>
   </si>
   <si>
@@ -87,9 +84,6 @@
     <t>Funciones Empresa</t>
   </si>
   <si>
-    <t>Acta Inicio</t>
-  </si>
-  <si>
     <t>F023_PC</t>
   </si>
   <si>
@@ -216,12 +210,6 @@
     <t>2023-01-01</t>
   </si>
   <si>
-    <t>2024-01-01</t>
-  </si>
-  <si>
-    <t>2024-07-01</t>
-  </si>
-  <si>
     <t>1900-01-01  PPRUEBA</t>
   </si>
   <si>
@@ -259,6 +247,21 @@
   </si>
   <si>
     <t>instructor_seguimiento</t>
+  </si>
+  <si>
+    <t>Alternativa(Equipo Etapa Productiva)</t>
+  </si>
+  <si>
+    <t>C.A.</t>
+  </si>
+  <si>
+    <t>V.L.</t>
+  </si>
+  <si>
+    <t>Pasantias</t>
+  </si>
+  <si>
+    <t>ActaInicio</t>
   </si>
 </sst>
 </file>
@@ -268,11 +271,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -356,16 +366,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -583,8 +595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BD1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -635,667 +647,673 @@
         <v>5</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AO1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AU1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AW1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AY1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AY1" s="2" t="s">
+      <c r="BA1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="BB1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="BC1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="BD1" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:56" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B2" s="1">
         <v>1112223</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="L2" s="6">
         <v>45474</v>
       </c>
       <c r="M2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="N2" s="10">
+        <f>EDATE(L2, 12)</f>
+        <v>45839</v>
+      </c>
+      <c r="O2" s="10">
+        <f>EDATE(L2, 18)</f>
+        <v>46023</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="R2" s="1">
         <f>COUNTIF(AA2:AM2, "si")</f>
         <v>3</v>
       </c>
       <c r="S2" s="8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>67</v>
+        <v>57</v>
+      </c>
+      <c r="Y2" s="9" t="s">
+        <v>68</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AG2" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AH2" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AI2" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AJ2" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AK2" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AL2" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AM2" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AN2" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AO2" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="AP2" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="AQ2" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AR2" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AS2" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AT2" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AU2" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AV2" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AW2" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AX2" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AY2" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AZ2" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="BA2" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="BB2" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="BC2" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="BD2" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B3" s="1">
         <v>1112223</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="G3" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="L3" s="6">
         <v>45474</v>
       </c>
       <c r="M3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="N3" s="10">
+        <f t="shared" ref="N3:N4" si="0">EDATE(L3, 12)</f>
+        <v>45839</v>
+      </c>
+      <c r="O3" s="10">
+        <f t="shared" ref="O3:O4" si="1">EDATE(L3, 18)</f>
+        <v>46023</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q3" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="O3" s="1" t="s">
+      <c r="R3" s="1">
+        <f t="shared" ref="R3:R4" si="2">COUNTIF(AA3:AM3, "si")</f>
+        <v>4</v>
+      </c>
+      <c r="S3" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE3" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF3" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AK3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AM3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AN3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AO3" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="AP3" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="Q3" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="R3" s="1">
-        <f t="shared" ref="R3:R4" si="0">COUNTIF(AA3:AM3, "si")</f>
-        <v>4</v>
-      </c>
-      <c r="S3" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y3" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA3" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="AB3" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="AC3" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="AD3" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="AE3" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="AF3" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="AG3" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AH3" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AI3" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AJ3" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AK3" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AL3" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AM3" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AN3" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AO3" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AP3" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="AQ3" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AR3" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AS3" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AT3" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AU3" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AV3" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AW3" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AX3" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AY3" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AZ3" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="BA3" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="BB3" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="BC3" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="BD3" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B4" s="1">
         <v>1112223</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="G4" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="L4" s="6">
         <v>45413</v>
       </c>
       <c r="M4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="N4" s="10">
+        <f t="shared" si="0"/>
+        <v>45778</v>
+      </c>
+      <c r="O4" s="10">
+        <f t="shared" si="1"/>
+        <v>45962</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q4" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="N4" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="O4" s="1" t="s">
+      <c r="R4" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S4" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y4" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AK4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AM4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AN4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AO4" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="AP4" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="Q4" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="R4" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="S4" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="X4" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y4" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="Z4" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA4" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB4" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="AC4" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="AD4" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="AE4" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="AF4" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="AG4" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AH4" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AI4" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AJ4" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AK4" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AL4" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AM4" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AN4" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AO4" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AP4" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="AQ4" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AR4" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AS4" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AT4" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AU4" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AV4" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AW4" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AX4" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AY4" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AZ4" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="BA4" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="BB4" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="BC4" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="BD4" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
se añade ficha para pruebas
se añade una ficha a la bd provisional para pruebas con alumnos
</commit_message>
<xml_diff>
--- a/Sources/prototiposSeguimiento.xlsx
+++ b/Sources/prototiposSeguimiento.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sena\Programacion de Software\Etapa productiva\requerimientosSenaBeta\requerimientosSenaBeta\Sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927EDA15-0F21-4641-B3F0-7B43A53D7EDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769894CD-2751-4F4D-AEDB-E3B276E55E5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -623,7 +623,7 @@
   <dimension ref="A1:BE4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -812,7 +812,7 @@
         <v>57</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>2782103</v>
       </c>
       <c r="E2" t="s">
         <v>76</v>

</xml_diff>

<commit_message>
Se actualiza correo para que le llegue al profe
se mete el correo hvelandia@sena.edu.co temporalmente para prueba de los alumnos
</commit_message>
<xml_diff>
--- a/Sources/prototiposSeguimiento.xlsx
+++ b/Sources/prototiposSeguimiento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sena\Programacion de Software\Etapa productiva\requerimientosSenaBeta\requerimientosSenaBeta\Sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769894CD-2751-4F4D-AEDB-E3B276E55E5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E74B4F9-9736-4151-9FE5-581F882488DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="79">
   <si>
     <t>TD</t>
   </si>
@@ -254,6 +254,9 @@
   </si>
   <si>
     <t>Tecnólogo</t>
+  </si>
+  <si>
+    <t>hvelandia@sena.edu.co</t>
   </si>
 </sst>
 </file>
@@ -623,7 +626,7 @@
   <dimension ref="A1:BE4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -857,7 +860,7 @@
         <v>3</v>
       </c>
       <c r="S2" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="Y2" t="s">
         <v>67</v>

</xml_diff>